<commit_message>
Colorisation, adaptation taille fenetre recherche
</commit_message>
<xml_diff>
--- a/suivi_jira_dcgf.xlsx
+++ b/suivi_jira_dcgf.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -585,6 +585,66 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>couleur</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>RAFALE</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Design plat ou les couleurs de l'interface utilisateur plats sont très populaires dans la conception web aujourd'hui où audacieuses, des couleurs vives sont utilisés pour créer des interfaces simples, propres</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Fermé</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>P2</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>couleur</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>RAFALE</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Design plat ou les couleurs de l'interface utilisateur plats sont très populaires dans la conception web aujourd'hui où audacieuses, des couleurs vives sont utilisés pour créer des interfaces simples, propres</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Ouvert</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>P3</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>